<commit_message>
20220608 复习paramiko openpyxl selenium
</commit_message>
<xml_diff>
--- a/B01_02 常用Python包学习/B01_02 10 Python_Excel/002 Docs/test1654591815.xlsx
+++ b/B01_02 常用Python包学习/B01_02 10 Python_Excel/002 Docs/test1654591815.xlsx
@@ -7,17 +7,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1号" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2号" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3号" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="4号" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="5号" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="6号" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="7号" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8号" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="9号" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="10号" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="11号" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第1号" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第2号" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第3号" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第4号" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第5号" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第6号" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第7号" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第8号" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第9号" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第10号" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="第11号" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>